<commit_message>
some more fixes for documentation
</commit_message>
<xml_diff>
--- a/output/endemo2_demand_projections.xlsx
+++ b/output/endemo2_demand_projections.xlsx
@@ -5507,15 +5507,27 @@
           <t>Portugal</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr"/>
-      <c r="C19" t="inlineStr"/>
+      <c r="B19" t="n">
+        <v>3.22</v>
+      </c>
+      <c r="C19" t="n">
+        <v>12.66</v>
+      </c>
       <c r="D19" t="n">
         <v>0</v>
       </c>
-      <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr"/>
-      <c r="G19" t="inlineStr"/>
-      <c r="H19" t="inlineStr"/>
+      <c r="E19" t="n">
+        <v>1.72</v>
+      </c>
+      <c r="F19" t="n">
+        <v>2.71</v>
+      </c>
+      <c r="G19" t="n">
+        <v>8.23</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0</v>
+      </c>
       <c r="I19" t="n">
         <v>100</v>
       </c>

</xml_diff>